<commit_message>
update files and add tree pdf
</commit_message>
<xml_diff>
--- a/WS Win Patterns.xlsx
+++ b/WS Win Patterns.xlsx
@@ -1,24 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gadamico/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5809ED-25CF-1048-94E6-F19E17B52B85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>GM 1</t>
   </si>
@@ -120,7 +130,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -162,6 +172,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -429,16 +442,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J114"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="H115" sqref="H115"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="K113" sqref="K113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="1" max="13" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -492,8 +505,8 @@
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
-        <v>8</v>
+      <c r="J2" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -512,11 +525,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
+      <c r="G3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H3" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -535,8 +548,8 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
-        <v>8</v>
+      <c r="H4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -558,11 +571,11 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>8</v>
+      <c r="G5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H5" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -581,11 +594,11 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
+      <c r="G6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -621,11 +634,11 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
-        <v>8</v>
+      <c r="G8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H8" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -644,8 +657,8 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
-        <v>8</v>
+      <c r="H9" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -684,11 +697,11 @@
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" t="s">
-        <v>8</v>
+      <c r="G11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H11" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -707,14 +720,14 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" t="s">
-        <v>8</v>
+      <c r="F12" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G12" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H12" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -733,11 +746,11 @@
       <c r="F13">
         <v>1</v>
       </c>
-      <c r="G13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" t="s">
-        <v>8</v>
+      <c r="G13" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H13" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -756,11 +769,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-      <c r="G14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" t="s">
-        <v>8</v>
+      <c r="G14" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H14" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -779,8 +792,8 @@
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="H15" t="s">
-        <v>8</v>
+      <c r="H15" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -799,8 +812,8 @@
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="H16" t="s">
-        <v>8</v>
+      <c r="H16" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -822,8 +835,8 @@
       <c r="I17">
         <v>1</v>
       </c>
-      <c r="J17" t="s">
-        <v>8</v>
+      <c r="J17" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -845,8 +858,11 @@
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="J18" t="s">
-        <v>8</v>
+      <c r="I18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J18" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -868,8 +884,8 @@
       <c r="I19">
         <v>1</v>
       </c>
-      <c r="J19" t="s">
-        <v>8</v>
+      <c r="J19" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -891,11 +907,11 @@
       <c r="F20">
         <v>1</v>
       </c>
-      <c r="G20" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" t="s">
-        <v>8</v>
+      <c r="G20" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H20" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -914,8 +930,8 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="H21" t="s">
-        <v>8</v>
+      <c r="H21" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -985,14 +1001,14 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" t="s">
-        <v>8</v>
+      <c r="F25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H25" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1011,14 +1027,14 @@
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" t="s">
-        <v>8</v>
+      <c r="F26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H26" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -1037,11 +1053,11 @@
       <c r="F27">
         <v>1</v>
       </c>
-      <c r="G27" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" t="s">
-        <v>8</v>
+      <c r="G27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H27" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1060,8 +1076,8 @@
       <c r="G28">
         <v>1</v>
       </c>
-      <c r="H28" t="s">
-        <v>8</v>
+      <c r="H28" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -1097,14 +1113,14 @@
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="F30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" t="s">
-        <v>8</v>
+      <c r="F30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H30" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -1123,11 +1139,11 @@
       <c r="F31">
         <v>1</v>
       </c>
-      <c r="G31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31" t="s">
-        <v>8</v>
+      <c r="G31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H31" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -1163,8 +1179,8 @@
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="H33" t="s">
-        <v>8</v>
+      <c r="H33" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1183,8 +1199,8 @@
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="H34" t="s">
-        <v>8</v>
+      <c r="H34" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1203,11 +1219,11 @@
       <c r="F35">
         <v>1</v>
       </c>
-      <c r="G35" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" t="s">
-        <v>8</v>
+      <c r="G35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H35" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1226,14 +1242,14 @@
       <c r="E36">
         <v>1</v>
       </c>
-      <c r="F36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" t="s">
-        <v>8</v>
+      <c r="F36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H36" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1252,14 +1268,14 @@
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" t="s">
-        <v>8</v>
-      </c>
-      <c r="H37" t="s">
-        <v>8</v>
+      <c r="F37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H37" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1295,11 +1311,11 @@
       <c r="F39">
         <v>1</v>
       </c>
-      <c r="G39" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39" t="s">
-        <v>8</v>
+      <c r="G39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H39" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1318,11 +1334,11 @@
       <c r="F40">
         <v>1</v>
       </c>
-      <c r="G40" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" t="s">
-        <v>8</v>
+      <c r="G40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H40" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1341,11 +1357,11 @@
       <c r="F41">
         <v>1</v>
       </c>
-      <c r="G41" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41" t="s">
-        <v>8</v>
+      <c r="G41" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H41" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1364,8 +1380,8 @@
       <c r="G42">
         <v>1</v>
       </c>
-      <c r="H42" t="s">
-        <v>8</v>
+      <c r="H42" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1435,8 +1451,8 @@
       <c r="G46">
         <v>1</v>
       </c>
-      <c r="H46" t="s">
-        <v>8</v>
+      <c r="H46" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1455,11 +1471,11 @@
       <c r="F47">
         <v>1</v>
       </c>
-      <c r="G47" t="s">
-        <v>8</v>
-      </c>
-      <c r="H47" t="s">
-        <v>8</v>
+      <c r="G47" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H47" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1478,14 +1494,14 @@
       <c r="E48">
         <v>1</v>
       </c>
-      <c r="F48" t="s">
-        <v>8</v>
-      </c>
-      <c r="G48" t="s">
-        <v>8</v>
-      </c>
-      <c r="H48" t="s">
-        <v>8</v>
+      <c r="F48" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G48" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H48" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1504,8 +1520,8 @@
       <c r="G49">
         <v>1</v>
       </c>
-      <c r="H49" t="s">
-        <v>8</v>
+      <c r="H49" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -1541,8 +1557,8 @@
       <c r="G51">
         <v>1</v>
       </c>
-      <c r="H51" t="s">
-        <v>8</v>
+      <c r="H51" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -1561,14 +1577,14 @@
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" t="s">
-        <v>8</v>
-      </c>
-      <c r="H52" t="s">
-        <v>8</v>
+      <c r="F52" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G52" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H52" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -1655,8 +1671,8 @@
       <c r="G57">
         <v>1</v>
       </c>
-      <c r="H57" t="s">
-        <v>8</v>
+      <c r="H57" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -1692,11 +1708,11 @@
       <c r="F59">
         <v>1</v>
       </c>
-      <c r="G59" t="s">
-        <v>8</v>
-      </c>
-      <c r="H59" t="s">
-        <v>8</v>
+      <c r="G59" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H59" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -1732,14 +1748,14 @@
       <c r="E61">
         <v>1</v>
       </c>
-      <c r="F61" t="s">
-        <v>8</v>
-      </c>
-      <c r="G61" t="s">
-        <v>8</v>
-      </c>
-      <c r="H61" t="s">
-        <v>8</v>
+      <c r="F61" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G61" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H61" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -1792,14 +1808,14 @@
       <c r="E64">
         <v>1</v>
       </c>
-      <c r="F64" t="s">
-        <v>8</v>
-      </c>
-      <c r="G64" t="s">
-        <v>8</v>
-      </c>
-      <c r="H64" t="s">
-        <v>8</v>
+      <c r="F64" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G64" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H64" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -1852,11 +1868,11 @@
       <c r="F67">
         <v>1</v>
       </c>
-      <c r="G67" t="s">
-        <v>8</v>
-      </c>
-      <c r="H67" t="s">
-        <v>8</v>
+      <c r="G67" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H67" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -1875,11 +1891,11 @@
       <c r="F68">
         <v>1</v>
       </c>
-      <c r="G68" t="s">
-        <v>8</v>
-      </c>
-      <c r="H68" t="s">
-        <v>8</v>
+      <c r="G68" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H68" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -1949,11 +1965,11 @@
       <c r="F72">
         <v>1</v>
       </c>
-      <c r="G72" t="s">
-        <v>8</v>
-      </c>
-      <c r="H72" t="s">
-        <v>8</v>
+      <c r="G72" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H72" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -1989,14 +2005,14 @@
       <c r="E74">
         <v>1</v>
       </c>
-      <c r="F74" t="s">
-        <v>8</v>
-      </c>
-      <c r="G74" t="s">
-        <v>8</v>
-      </c>
-      <c r="H74" t="s">
-        <v>8</v>
+      <c r="F74" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G74" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H74" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -2015,8 +2031,8 @@
       <c r="G75">
         <v>1</v>
       </c>
-      <c r="H75" t="s">
-        <v>8</v>
+      <c r="H75" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2035,8 +2051,8 @@
       <c r="G76">
         <v>1</v>
       </c>
-      <c r="H76" t="s">
-        <v>8</v>
+      <c r="H76" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2072,8 +2088,8 @@
       <c r="G78">
         <v>1</v>
       </c>
-      <c r="H78" t="s">
-        <v>8</v>
+      <c r="H78" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2092,8 +2108,8 @@
       <c r="G79">
         <v>1</v>
       </c>
-      <c r="H79" t="s">
-        <v>8</v>
+      <c r="H79" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2129,11 +2145,11 @@
       <c r="F81">
         <v>1</v>
       </c>
-      <c r="G81" t="s">
-        <v>8</v>
-      </c>
-      <c r="H81" t="s">
-        <v>8</v>
+      <c r="G81" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H81" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2152,11 +2168,11 @@
       <c r="F82">
         <v>1</v>
       </c>
-      <c r="G82" t="s">
-        <v>8</v>
-      </c>
-      <c r="H82" t="s">
-        <v>8</v>
+      <c r="G82" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H82" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2226,11 +2242,11 @@
       <c r="F86">
         <v>1</v>
       </c>
-      <c r="G86" t="s">
-        <v>8</v>
-      </c>
-      <c r="H86" t="s">
-        <v>8</v>
+      <c r="G86" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H86" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -2249,14 +2265,14 @@
       <c r="E87">
         <v>1</v>
       </c>
-      <c r="F87" t="s">
-        <v>8</v>
-      </c>
-      <c r="G87" t="s">
-        <v>8</v>
-      </c>
-      <c r="H87" t="s">
-        <v>8</v>
+      <c r="F87" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G87" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H87" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -2275,14 +2291,14 @@
       <c r="E88">
         <v>1</v>
       </c>
-      <c r="F88" t="s">
-        <v>8</v>
-      </c>
-      <c r="G88" t="s">
-        <v>8</v>
-      </c>
-      <c r="H88" t="s">
-        <v>8</v>
+      <c r="F88" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G88" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H88" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -2318,8 +2334,8 @@
       <c r="G90">
         <v>1</v>
       </c>
-      <c r="H90" t="s">
-        <v>8</v>
+      <c r="H90" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -2338,8 +2354,8 @@
       <c r="G91">
         <v>1</v>
       </c>
-      <c r="H91" t="s">
-        <v>8</v>
+      <c r="H91" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -2358,8 +2374,8 @@
       <c r="G92">
         <v>1</v>
       </c>
-      <c r="H92" t="s">
-        <v>8</v>
+      <c r="H92" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -2378,8 +2394,8 @@
       <c r="G93">
         <v>1</v>
       </c>
-      <c r="H93" t="s">
-        <v>8</v>
+      <c r="H93" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -2415,14 +2431,14 @@
       <c r="E95">
         <v>1</v>
       </c>
-      <c r="F95" t="s">
-        <v>8</v>
-      </c>
-      <c r="G95" t="s">
-        <v>8</v>
-      </c>
-      <c r="H95" t="s">
-        <v>8</v>
+      <c r="F95" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G95" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H95" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -2441,17 +2457,17 @@
       <c r="E96">
         <v>1</v>
       </c>
-      <c r="F96" t="s">
-        <v>8</v>
-      </c>
-      <c r="G96" t="s">
-        <v>8</v>
-      </c>
-      <c r="H96" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F96" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G96" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H96" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2000</v>
       </c>
@@ -2467,14 +2483,14 @@
       <c r="F97">
         <v>1</v>
       </c>
-      <c r="G97" t="s">
-        <v>8</v>
-      </c>
-      <c r="H97" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G97" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H97" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2001</v>
       </c>
@@ -2491,7 +2507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2002</v>
       </c>
@@ -2508,7 +2524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2003</v>
       </c>
@@ -2524,11 +2540,11 @@
       <c r="G100">
         <v>1</v>
       </c>
-      <c r="H100" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H100" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2004</v>
       </c>
@@ -2544,17 +2560,17 @@
       <c r="E101">
         <v>1</v>
       </c>
-      <c r="F101" t="s">
-        <v>8</v>
-      </c>
-      <c r="G101" t="s">
-        <v>8</v>
-      </c>
-      <c r="H101" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F101" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G101" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H101" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2005</v>
       </c>
@@ -2570,17 +2586,17 @@
       <c r="E102">
         <v>1</v>
       </c>
-      <c r="F102" t="s">
-        <v>8</v>
-      </c>
-      <c r="G102" t="s">
-        <v>8</v>
-      </c>
-      <c r="H102" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F102" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G102" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H102" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2006</v>
       </c>
@@ -2596,14 +2612,14 @@
       <c r="F103">
         <v>1</v>
       </c>
-      <c r="G103" t="s">
-        <v>8</v>
-      </c>
-      <c r="H103" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G103" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H103" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2007</v>
       </c>
@@ -2619,17 +2635,17 @@
       <c r="E104">
         <v>1</v>
       </c>
-      <c r="F104" t="s">
-        <v>8</v>
-      </c>
-      <c r="G104" t="s">
-        <v>8</v>
-      </c>
-      <c r="H104" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F104" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G104" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H104" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2008</v>
       </c>
@@ -2645,14 +2661,14 @@
       <c r="F105">
         <v>1</v>
       </c>
-      <c r="G105" t="s">
-        <v>8</v>
-      </c>
-      <c r="H105" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G105" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H105" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2009</v>
       </c>
@@ -2668,11 +2684,11 @@
       <c r="G106">
         <v>1</v>
       </c>
-      <c r="H106" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H106" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2010</v>
       </c>
@@ -2688,14 +2704,14 @@
       <c r="F107">
         <v>1</v>
       </c>
-      <c r="G107" t="s">
-        <v>8</v>
-      </c>
-      <c r="H107" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G107" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H107" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2011</v>
       </c>
@@ -2712,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>2012</v>
       </c>
@@ -2728,17 +2744,17 @@
       <c r="E109">
         <v>1</v>
       </c>
-      <c r="F109" t="s">
-        <v>8</v>
-      </c>
-      <c r="G109" t="s">
-        <v>8</v>
-      </c>
-      <c r="H109" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F109" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G109" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H109" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>2013</v>
       </c>
@@ -2754,11 +2770,11 @@
       <c r="G110">
         <v>1</v>
       </c>
-      <c r="H110" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H110" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2014</v>
       </c>
@@ -2775,7 +2791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>2015</v>
       </c>
@@ -2791,14 +2807,26 @@
       <c r="F112">
         <v>1</v>
       </c>
-      <c r="G112" t="s">
-        <v>8</v>
-      </c>
-      <c r="H112" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G112" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H112" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J112">
+        <f xml:space="preserve"> ROUND(((SUM(E3:E4) + SUM(E6:E9) + SUM(E11:E16) + SUM(E21:E116) - (J113 - K113))/K113), 3)</f>
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="K112">
+        <f xml:space="preserve"> ROUND(((SUMIF(F3:F4, "&lt;&gt;#N/A") + SUMIF(F6:F9, "&lt;&gt;#N/A") + SUMIF(F11:F16, "&lt;&gt;#N/A") + SUMIF(F21:F116, "&lt;&gt;#N/A") - (K113 - L113)) / L113), 3)</f>
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="L112">
+        <f>ROUND(((SUMIF(G3:G4, "&lt;&gt;#N/A") + SUMIF(G6:G9, "&lt;&gt;#N/A") + SUMIF(G11:G16, "&lt;&gt;#N/A") + SUMIF(G21:G116, "&lt;&gt;#N/A") - (L113 - M113)) / M113), 3)</f>
+        <v>0.53800000000000003</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>2016</v>
       </c>
@@ -2814,37 +2842,129 @@
       <c r="H113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="J113">
+        <v>109</v>
+      </c>
+      <c r="K113">
+        <f xml:space="preserve"> J113 - (COUNTIF(F3:F4, #N/A) + COUNTIF(F6:F9, #N/A) + COUNTIF(F11:F16, #N/A) + COUNTIF(F21:F117, #N/A))</f>
+        <v>90</v>
+      </c>
+      <c r="L113">
+        <f xml:space="preserve"> J113 - (COUNTIF(G3:G4, #N/A) + COUNTIF(G6:G9, #N/A) + COUNTIF(G11:G16, #N/A) + COUNTIF(G21:G117, #N/A))</f>
+        <v>64</v>
+      </c>
+      <c r="M113">
+        <f xml:space="preserve"> J113 - (COUNTIF(H3:H4, #N/A) + COUNTIF(H6:H9, #N/A) + COUNTIF(H11:H16, #N/A) + COUNTIF(H21:H117, #N/A))</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>2017</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <v>1</v>
+      </c>
+      <c r="H114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>2018</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <v>1</v>
+      </c>
+      <c r="G115" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H115" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>2019</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="G116">
+        <v>1</v>
+      </c>
+      <c r="H116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>2020</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <v>1</v>
+      </c>
+      <c r="G117">
+        <v>1</v>
+      </c>
+      <c r="H117" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>27</v>
       </c>
-      <c r="B114">
-        <f>(SUM(B3:B4) + SUM(B6:B9) + SUM(B11:B16) + SUM(B21:B113))/105</f>
-        <v>0.62857142857142856</v>
-      </c>
-      <c r="C114">
-        <f>(SUM(C3:C4) + SUM(C6:C9) + SUM(C11:C16) + SUM(C21:C113))/105</f>
-        <v>0.65714285714285714</v>
-      </c>
-      <c r="D114">
-        <f>(SUM(D3:D4) + SUM(D6:D9) + SUM(D11:D16) + SUM(D21:D113))/105</f>
-        <v>0.65714285714285714</v>
-      </c>
-      <c r="E114">
-        <f>(SUM(E3:E4) + SUM(E6:E9) + SUM(E11:E16) + SUM(E21:E113))/105</f>
-        <v>0.72380952380952379</v>
-      </c>
-      <c r="F114">
-        <f xml:space="preserve"> (SUM(F3:F4) + SUM(F6:F9) + SUM(F11:F16) + SUM(F21:F113))/86</f>
-        <v>0.67441860465116277</v>
-      </c>
-      <c r="G114">
-        <f>(SUM(G3:G4) + SUM(G6:G9) + SUM(G11:G16) + SUM(G21:G113))/61</f>
-        <v>0.73770491803278693</v>
-      </c>
-      <c r="H114">
-        <f>(SUM(H3:H4) + SUM(H6:H9) + SUM(H11:H16) + SUM(H21:H113))/37</f>
+      <c r="B118">
+        <f xml:space="preserve"> ROUND(((SUM(B3:B4) + SUM(B6:B9) + SUM(B11:B16) + SUM(B21:B117))/J113), 3)</f>
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="C118">
+        <f xml:space="preserve"> ROUND(((SUM(C3:C4) + SUM(C6:C9) + SUM(C11:C16) + SUM(C21:C117))/J113), 3)</f>
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="D118">
+        <f xml:space="preserve"> ROUND(((SUM(D3:D4) + SUM(D6:D9) + SUM(D11:D16) + SUM(D21:D117))/J113), 3)</f>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="E118">
+        <f xml:space="preserve"> ROUND(((SUM(E3:E4) + SUM(E6:E9) + SUM(E11:E16) + SUM(E21:E117))/J113), 3)</f>
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="F118">
+        <f xml:space="preserve"> ROUND(((SUMIF(F3:F4, "&lt;&gt;#N/A") + SUMIF(F6:F9, "&lt;&gt;#N/A") + SUMIF(F11:F16, "&lt;&gt;#N/A") + SUMIF(F21:F117, "&lt;&gt;#N/A"))/K113), 3)</f>
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="G118">
+        <f xml:space="preserve"> ROUND(((SUMIF(G3:G4, "&lt;&gt;#N/A") + SUMIF(G6:G9, "&lt;&gt;#N/A") + SUMIF(G11:G16, "&lt;&gt;#N/A") + SUMIF(G21:G117, "&lt;&gt;#N/A"))/L113), 3)</f>
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="H118">
+        <f xml:space="preserve"> ROUND(((SUMIF(H3:H4, "&lt;&gt;#N/A") + SUMIF(H6:H9, "&lt;&gt;#N/A") + SUMIF(H11:H16, "&lt;&gt;#N/A") + SUMIF(H21:H117, "&lt;&gt;#N/A"))/M113), 2)</f>
         <v>1</v>
       </c>
     </row>
@@ -2854,11 +2974,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2956,7 +3076,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3050,23 +3170,17 @@
       <c r="B8">
         <v>4</v>
       </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" t="s">
-        <v>8</v>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3076,6 +3190,9 @@
       <c r="B9">
         <v>4</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="E9">
         <v>1</v>
       </c>
@@ -3085,8 +3202,11 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="I9">
-        <v>1</v>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -3111,33 +3231,27 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" t="s">
-        <v>8</v>
+      <c r="I11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -3148,16 +3262,22 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -3180,7 +3300,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -3200,7 +3320,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -3220,7 +3340,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -3240,7 +3360,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -3251,7 +3371,7 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="H17">
+      <c r="G17">
         <v>1</v>
       </c>
       <c r="I17">
@@ -3260,7 +3380,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -3268,27 +3388,24 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
+      <c r="E18">
         <v>1</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18" t="s">
-        <v>8</v>
+      <c r="I18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
-      <c r="E19">
+      <c r="D19">
         <v>1</v>
       </c>
       <c r="F19">
@@ -3306,12 +3423,12 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="E20">
         <v>1</v>
       </c>
       <c r="F20">
@@ -3329,12 +3446,12 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
-      <c r="D21">
+      <c r="C21">
         <v>1</v>
       </c>
       <c r="E21">
@@ -3343,18 +3460,24 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="I21">
-        <v>1</v>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
-      <c r="E22">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
@@ -3363,36 +3486,33 @@
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22">
-        <v>1</v>
+      <c r="I22" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="G23">
         <v>1</v>
       </c>
       <c r="H23">
         <v>1</v>
       </c>
-      <c r="I23" t="s">
-        <v>8</v>
+      <c r="I23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3406,13 +3526,16 @@
       <c r="F24">
         <v>1</v>
       </c>
-      <c r="I24">
-        <v>1</v>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3423,7 +3546,7 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="G25">
+      <c r="F25">
         <v>1</v>
       </c>
       <c r="I25">
@@ -3432,7 +3555,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3440,10 +3563,10 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="G26">
         <v>1</v>
       </c>
       <c r="I26">
@@ -3452,7 +3575,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3463,19 +3586,16 @@
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27" t="s">
-        <v>8</v>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3495,7 +3615,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3660,6 +3780,15 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I36">
+    <sortCondition descending="1" ref="B2:B36"/>
+    <sortCondition descending="1" ref="C2:C36"/>
+    <sortCondition descending="1" ref="D2:D36"/>
+    <sortCondition descending="1" ref="E2:E36"/>
+    <sortCondition descending="1" ref="F2:F36"/>
+    <sortCondition descending="1" ref="G2:G36"/>
+    <sortCondition descending="1" ref="H2:H36"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>